<commit_message>
Perubahan pada query page Kinerja menambahkan data spesifik tahun 2021 dan update data excel kinerja 2021
</commit_message>
<xml_diff>
--- a/public/uploads/Kinerja 2021 PLTD Kotamobagu.xlsx
+++ b/public/uploads/Kinerja 2021 PLTD Kotamobagu.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Coding\Mongodb\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Website Projects\Latihan Project\portal-pltd-kotamobagu\public\uploads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{228E7325-E972-42BE-ABCE-F0F6256A9EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D70D3D82-EE1E-4F96-84BE-12E1BCAB61A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{26EA7E96-9E20-490C-B7F9-A388545D0051}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{26EA7E96-9E20-490C-B7F9-A388545D0051}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -276,9 +276,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>744</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -326,9 +323,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>744</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -376,9 +370,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>744</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -426,9 +417,6 @@
           <cell r="X59">
             <v>0</v>
           </cell>
-          <cell r="Z59">
-            <v>744</v>
-          </cell>
           <cell r="AA59">
             <v>0</v>
           </cell>
@@ -476,9 +464,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>744</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -526,43 +511,10 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>744</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
           <cell r="AB61">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="62">
-          <cell r="Z62">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="63">
-          <cell r="Z63">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="64">
-          <cell r="Z64">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="65">
-          <cell r="Z65">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="66">
-          <cell r="Z66">
-            <v>0</v>
-          </cell>
-        </row>
-        <row r="67">
-          <cell r="Z67">
             <v>0</v>
           </cell>
         </row>
@@ -608,9 +560,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>672</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -658,9 +607,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>672</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -708,9 +654,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>672</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -758,9 +701,6 @@
           <cell r="X59">
             <v>0</v>
           </cell>
-          <cell r="Z59">
-            <v>672</v>
-          </cell>
           <cell r="AA59">
             <v>0</v>
           </cell>
@@ -808,9 +748,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>672</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -858,9 +795,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>672</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -899,9 +833,6 @@
           <cell r="T62">
             <v>101.52000000000044</v>
           </cell>
-          <cell r="Z62">
-            <v>672</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -940,9 +871,6 @@
           <cell r="T63">
             <v>88.25</v>
           </cell>
-          <cell r="Z63">
-            <v>672</v>
-          </cell>
           <cell r="AA63">
             <v>1</v>
           </cell>
@@ -981,9 +909,6 @@
           <cell r="T64">
             <v>92.349999999998545</v>
           </cell>
-          <cell r="Z64">
-            <v>672</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -1022,9 +947,6 @@
           <cell r="T65">
             <v>94.989999999999782</v>
           </cell>
-          <cell r="Z65">
-            <v>672</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -1063,9 +985,6 @@
           <cell r="T66">
             <v>102.35000000000036</v>
           </cell>
-          <cell r="Z66">
-            <v>672</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -1103,9 +1022,6 @@
           </cell>
           <cell r="T67">
             <v>95.159999999999854</v>
-          </cell>
-          <cell r="Z67">
-            <v>672</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -1157,9 +1073,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>744</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -1207,9 +1120,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>744</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -1257,9 +1167,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>744</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -1307,9 +1214,6 @@
           <cell r="X59">
             <v>0</v>
           </cell>
-          <cell r="Z59">
-            <v>744</v>
-          </cell>
           <cell r="AA59">
             <v>0</v>
           </cell>
@@ -1357,9 +1261,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>744</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -1407,9 +1308,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>744</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -1457,9 +1355,6 @@
           <cell r="X62">
             <v>0</v>
           </cell>
-          <cell r="Z62">
-            <v>744</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -1507,9 +1402,6 @@
           <cell r="X63">
             <v>0</v>
           </cell>
-          <cell r="Z63">
-            <v>744</v>
-          </cell>
           <cell r="AA63">
             <v>0</v>
           </cell>
@@ -1557,9 +1449,6 @@
           <cell r="X64">
             <v>0</v>
           </cell>
-          <cell r="Z64">
-            <v>744</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -1607,9 +1496,6 @@
           <cell r="X65">
             <v>0</v>
           </cell>
-          <cell r="Z65">
-            <v>744</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -1657,9 +1543,6 @@
           <cell r="X66">
             <v>0</v>
           </cell>
-          <cell r="Z66">
-            <v>744</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -1706,9 +1589,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>744</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -1760,9 +1640,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>720</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -1810,9 +1687,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>720</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -1860,9 +1734,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>720</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -1910,9 +1781,6 @@
           <cell r="X59">
             <v>0</v>
           </cell>
-          <cell r="Z59">
-            <v>0</v>
-          </cell>
           <cell r="AA59">
             <v>0</v>
           </cell>
@@ -1960,9 +1828,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>720</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -2010,9 +1875,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>720</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -2060,9 +1922,6 @@
           <cell r="X62">
             <v>0</v>
           </cell>
-          <cell r="Z62">
-            <v>720</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -2110,9 +1969,6 @@
           <cell r="X63">
             <v>0</v>
           </cell>
-          <cell r="Z63">
-            <v>720</v>
-          </cell>
           <cell r="AA63">
             <v>0</v>
           </cell>
@@ -2160,9 +2016,6 @@
           <cell r="X64">
             <v>0</v>
           </cell>
-          <cell r="Z64">
-            <v>720</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -2210,9 +2063,6 @@
           <cell r="X65">
             <v>0</v>
           </cell>
-          <cell r="Z65">
-            <v>720</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -2260,9 +2110,6 @@
           <cell r="X66">
             <v>0</v>
           </cell>
-          <cell r="Z66">
-            <v>720</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -2309,9 +2156,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>720</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -2363,9 +2207,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>744</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -2413,9 +2254,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>744</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -2463,9 +2301,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>744</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -2513,9 +2348,6 @@
           <cell r="X59">
             <v>0</v>
           </cell>
-          <cell r="Z59">
-            <v>0</v>
-          </cell>
           <cell r="AA59">
             <v>0</v>
           </cell>
@@ -2563,9 +2395,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>744</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -2613,9 +2442,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>744</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -2663,9 +2489,6 @@
           <cell r="X62">
             <v>0</v>
           </cell>
-          <cell r="Z62">
-            <v>744</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -2713,9 +2536,6 @@
           <cell r="X63">
             <v>0</v>
           </cell>
-          <cell r="Z63">
-            <v>744</v>
-          </cell>
           <cell r="AA63">
             <v>0</v>
           </cell>
@@ -2763,9 +2583,6 @@
           <cell r="X64">
             <v>0</v>
           </cell>
-          <cell r="Z64">
-            <v>744</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -2813,9 +2630,6 @@
           <cell r="X65">
             <v>0</v>
           </cell>
-          <cell r="Z65">
-            <v>744</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -2863,9 +2677,6 @@
           <cell r="X66">
             <v>0</v>
           </cell>
-          <cell r="Z66">
-            <v>744</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -2912,9 +2723,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>744</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -2966,9 +2774,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>720</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -3016,9 +2821,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>720</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -3066,9 +2868,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>720</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -3114,9 +2913,6 @@
             <v>0</v>
           </cell>
           <cell r="X59">
-            <v>0</v>
-          </cell>
-          <cell r="Z59">
             <v>0</v>
           </cell>
           <cell r="AA59">
@@ -3166,9 +2962,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>720</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -3216,9 +3009,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>720</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -3266,9 +3056,6 @@
           <cell r="X62">
             <v>0</v>
           </cell>
-          <cell r="Z62">
-            <v>720</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -3316,9 +3103,6 @@
           <cell r="X63">
             <v>0</v>
           </cell>
-          <cell r="Z63">
-            <v>720</v>
-          </cell>
           <cell r="AA63">
             <v>0</v>
           </cell>
@@ -3366,9 +3150,6 @@
           <cell r="X64">
             <v>0</v>
           </cell>
-          <cell r="Z64">
-            <v>720</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -3416,9 +3197,6 @@
           <cell r="X65">
             <v>0</v>
           </cell>
-          <cell r="Z65">
-            <v>720</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -3466,9 +3244,6 @@
           <cell r="X66">
             <v>0</v>
           </cell>
-          <cell r="Z66">
-            <v>720</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -3515,9 +3290,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>720</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -3569,9 +3341,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>744</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -3619,9 +3388,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>744</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -3669,9 +3435,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>744</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -3717,9 +3480,6 @@
             <v>0</v>
           </cell>
           <cell r="X59">
-            <v>0</v>
-          </cell>
-          <cell r="Z59">
             <v>0</v>
           </cell>
           <cell r="AA59">
@@ -3769,9 +3529,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>744</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -3819,9 +3576,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>744</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -3869,9 +3623,6 @@
           <cell r="X62">
             <v>0</v>
           </cell>
-          <cell r="Z62">
-            <v>744</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -3919,9 +3670,6 @@
           <cell r="X63">
             <v>0</v>
           </cell>
-          <cell r="Z63">
-            <v>744</v>
-          </cell>
           <cell r="AA63">
             <v>0</v>
           </cell>
@@ -3969,9 +3717,6 @@
           <cell r="X64">
             <v>0</v>
           </cell>
-          <cell r="Z64">
-            <v>744</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -4019,9 +3764,6 @@
           <cell r="X65">
             <v>0</v>
           </cell>
-          <cell r="Z65">
-            <v>744</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -4069,9 +3811,6 @@
           <cell r="X66">
             <v>0</v>
           </cell>
-          <cell r="Z66">
-            <v>744</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -4118,9 +3857,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>744</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -4172,9 +3908,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>744</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -4222,9 +3955,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>744</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -4272,9 +4002,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>744</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -4320,9 +4047,6 @@
             <v>0</v>
           </cell>
           <cell r="X59">
-            <v>0</v>
-          </cell>
-          <cell r="Z59">
             <v>0</v>
           </cell>
           <cell r="AA59">
@@ -4372,9 +4096,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>744</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -4422,9 +4143,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>744</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -4472,9 +4190,6 @@
           <cell r="X62">
             <v>0</v>
           </cell>
-          <cell r="Z62">
-            <v>744</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -4522,9 +4237,6 @@
           <cell r="X63">
             <v>0</v>
           </cell>
-          <cell r="Z63">
-            <v>744</v>
-          </cell>
           <cell r="AA63">
             <v>0</v>
           </cell>
@@ -4572,9 +4284,6 @@
           <cell r="X64">
             <v>0</v>
           </cell>
-          <cell r="Z64">
-            <v>744</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -4622,9 +4331,6 @@
           <cell r="X65">
             <v>0</v>
           </cell>
-          <cell r="Z65">
-            <v>744</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -4672,9 +4378,6 @@
           <cell r="X66">
             <v>0</v>
           </cell>
-          <cell r="Z66">
-            <v>744</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -4721,9 +4424,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>744</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -4775,9 +4475,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>720</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -4825,9 +4522,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>720</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -4875,9 +4569,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>720</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -4923,9 +4614,6 @@
             <v>0</v>
           </cell>
           <cell r="X59">
-            <v>0</v>
-          </cell>
-          <cell r="Z59">
             <v>0</v>
           </cell>
           <cell r="AA59">
@@ -4975,9 +4663,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>720</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -5025,9 +4710,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>720</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -5075,9 +4757,6 @@
           <cell r="X62">
             <v>0</v>
           </cell>
-          <cell r="Z62">
-            <v>720</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -5125,9 +4804,6 @@
           <cell r="X63">
             <v>0</v>
           </cell>
-          <cell r="Z63">
-            <v>720</v>
-          </cell>
           <cell r="AA63">
             <v>0</v>
           </cell>
@@ -5175,9 +4851,6 @@
           <cell r="X64">
             <v>0</v>
           </cell>
-          <cell r="Z64">
-            <v>720</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -5225,9 +4898,6 @@
           <cell r="X65">
             <v>0</v>
           </cell>
-          <cell r="Z65">
-            <v>720</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -5275,9 +4945,6 @@
           <cell r="X66">
             <v>0</v>
           </cell>
-          <cell r="Z66">
-            <v>720</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -5324,9 +4991,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>720</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -5378,9 +5042,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>744</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -5428,9 +5089,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>744</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -5478,9 +5136,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>744</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -5526,9 +5181,6 @@
             <v>0</v>
           </cell>
           <cell r="X59">
-            <v>0</v>
-          </cell>
-          <cell r="Z59">
             <v>0</v>
           </cell>
           <cell r="AA59">
@@ -5578,9 +5230,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>744</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -5628,9 +5277,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>744</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -5678,9 +5324,6 @@
           <cell r="X62">
             <v>0</v>
           </cell>
-          <cell r="Z62">
-            <v>744</v>
-          </cell>
           <cell r="AA62">
             <v>0</v>
           </cell>
@@ -5728,9 +5371,6 @@
           <cell r="X63">
             <v>0</v>
           </cell>
-          <cell r="Z63">
-            <v>744</v>
-          </cell>
           <cell r="AA63">
             <v>0</v>
           </cell>
@@ -5778,9 +5418,6 @@
           <cell r="X64">
             <v>0</v>
           </cell>
-          <cell r="Z64">
-            <v>744</v>
-          </cell>
           <cell r="AA64">
             <v>0</v>
           </cell>
@@ -5828,9 +5465,6 @@
           <cell r="X65">
             <v>0</v>
           </cell>
-          <cell r="Z65">
-            <v>744</v>
-          </cell>
           <cell r="AA65">
             <v>0</v>
           </cell>
@@ -5878,9 +5512,6 @@
           <cell r="X66">
             <v>0</v>
           </cell>
-          <cell r="Z66">
-            <v>744</v>
-          </cell>
           <cell r="AA66">
             <v>0</v>
           </cell>
@@ -5927,9 +5558,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>744</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -5949,16 +5577,16 @@
             <v>300</v>
           </cell>
           <cell r="J56">
-            <v>0</v>
+            <v>220</v>
           </cell>
           <cell r="K56">
-            <v>0</v>
+            <v>9.0000000000009095</v>
           </cell>
           <cell r="L56">
-            <v>0</v>
+            <v>3.52</v>
           </cell>
           <cell r="N56">
-            <v>0</v>
+            <v>116</v>
           </cell>
           <cell r="P56">
             <v>0</v>
@@ -5970,7 +5598,7 @@
             <v>0</v>
           </cell>
           <cell r="T56">
-            <v>0</v>
+            <v>1.1000000000000014</v>
           </cell>
           <cell r="V56">
             <v>0</v>
@@ -5980,9 +5608,6 @@
           </cell>
           <cell r="X56">
             <v>0</v>
-          </cell>
-          <cell r="Z56">
-            <v>744</v>
           </cell>
           <cell r="AA56">
             <v>0</v>
@@ -5999,16 +5624,16 @@
             <v>350</v>
           </cell>
           <cell r="J57">
-            <v>0</v>
+            <v>3330</v>
           </cell>
           <cell r="K57">
-            <v>0</v>
+            <v>224</v>
           </cell>
           <cell r="L57">
-            <v>0</v>
+            <v>53.28</v>
           </cell>
           <cell r="N57">
-            <v>0</v>
+            <v>1286</v>
           </cell>
           <cell r="P57">
             <v>0</v>
@@ -6020,7 +5645,7 @@
             <v>0</v>
           </cell>
           <cell r="T57">
-            <v>0</v>
+            <v>14.666666666666664</v>
           </cell>
           <cell r="V57">
             <v>0</v>
@@ -6030,9 +5655,6 @@
           </cell>
           <cell r="X57">
             <v>0</v>
-          </cell>
-          <cell r="Z57">
-            <v>744</v>
           </cell>
           <cell r="AA57">
             <v>0</v>
@@ -6052,7 +5674,7 @@
             <v>0</v>
           </cell>
           <cell r="K58">
-            <v>0</v>
+            <v>7.9999999998835847</v>
           </cell>
           <cell r="L58">
             <v>0</v>
@@ -6080,9 +5702,6 @@
           </cell>
           <cell r="X58">
             <v>0</v>
-          </cell>
-          <cell r="Z58">
-            <v>744</v>
           </cell>
           <cell r="AA58">
             <v>0</v>
@@ -6129,9 +5748,6 @@
             <v>0</v>
           </cell>
           <cell r="X59">
-            <v>0</v>
-          </cell>
-          <cell r="Z59">
             <v>0</v>
           </cell>
           <cell r="AA59">
@@ -6149,16 +5765,16 @@
             <v>2000</v>
           </cell>
           <cell r="J60">
-            <v>34370</v>
+            <v>31950</v>
           </cell>
           <cell r="K60">
-            <v>1026</v>
+            <v>970</v>
           </cell>
           <cell r="L60">
-            <v>549.91999999999996</v>
+            <v>511.2</v>
           </cell>
           <cell r="N60">
-            <v>9511</v>
+            <v>8825</v>
           </cell>
           <cell r="P60">
             <v>0</v>
@@ -6170,7 +5786,7 @@
             <v>0</v>
           </cell>
           <cell r="T60">
-            <v>22.383333333333329</v>
+            <v>21.483333333333345</v>
           </cell>
           <cell r="V60">
             <v>0</v>
@@ -6180,9 +5796,6 @@
           </cell>
           <cell r="X60">
             <v>0</v>
-          </cell>
-          <cell r="Z60">
-            <v>744</v>
           </cell>
           <cell r="AA60">
             <v>0</v>
@@ -6199,16 +5812,16 @@
             <v>1900</v>
           </cell>
           <cell r="J61">
-            <v>31150</v>
+            <v>25240</v>
           </cell>
           <cell r="K61">
-            <v>1046</v>
+            <v>902</v>
           </cell>
           <cell r="L61">
-            <v>498.40000000000003</v>
+            <v>403.84000000000003</v>
           </cell>
           <cell r="N61">
-            <v>8363</v>
+            <v>6926</v>
           </cell>
           <cell r="P61">
             <v>0</v>
@@ -6220,7 +5833,7 @@
             <v>0</v>
           </cell>
           <cell r="T61">
-            <v>21.79999999999999</v>
+            <v>18.733333333333334</v>
           </cell>
           <cell r="V61">
             <v>0</v>
@@ -6230,9 +5843,6 @@
           </cell>
           <cell r="X61">
             <v>0</v>
-          </cell>
-          <cell r="Z61">
-            <v>744</v>
           </cell>
           <cell r="AA61">
             <v>0</v>
@@ -6249,16 +5859,16 @@
             <v>1000</v>
           </cell>
           <cell r="J62">
-            <v>0</v>
+            <v>10802.599999999627</v>
           </cell>
           <cell r="K62">
-            <v>0</v>
+            <v>58.900000000372529</v>
           </cell>
           <cell r="L62">
-            <v>0</v>
+            <v>243.69999999925494</v>
           </cell>
           <cell r="N62">
-            <v>0</v>
+            <v>3103.0000000000459</v>
           </cell>
           <cell r="P62">
             <v>0</v>
@@ -6270,7 +5880,7 @@
             <v>0</v>
           </cell>
           <cell r="T62">
-            <v>0</v>
+            <v>12.049999999999272</v>
           </cell>
           <cell r="V62">
             <v>0</v>
@@ -6280,9 +5890,6 @@
           </cell>
           <cell r="X62">
             <v>0</v>
-          </cell>
-          <cell r="Z62">
-            <v>744</v>
           </cell>
           <cell r="AA62">
             <v>0</v>
@@ -6299,16 +5906,16 @@
             <v>1000</v>
           </cell>
           <cell r="J63">
-            <v>0</v>
+            <v>11934.400000000373</v>
           </cell>
           <cell r="K63">
-            <v>0</v>
+            <v>138.19999999925494</v>
           </cell>
           <cell r="L63">
-            <v>0</v>
+            <v>496.20000000184518</v>
           </cell>
           <cell r="N63">
-            <v>0</v>
+            <v>3467.000000000517</v>
           </cell>
           <cell r="P63">
             <v>0</v>
@@ -6320,7 +5927,7 @@
             <v>0</v>
           </cell>
           <cell r="T63">
-            <v>0</v>
+            <v>13.329999999999927</v>
           </cell>
           <cell r="V63">
             <v>0</v>
@@ -6330,9 +5937,6 @@
           </cell>
           <cell r="X63">
             <v>0</v>
-          </cell>
-          <cell r="Z63">
-            <v>744</v>
           </cell>
           <cell r="AA63">
             <v>0</v>
@@ -6349,16 +5953,16 @@
             <v>1000</v>
           </cell>
           <cell r="J64">
-            <v>0</v>
+            <v>12485.599999999627</v>
           </cell>
           <cell r="K64">
-            <v>0</v>
+            <v>157.29999999888241</v>
           </cell>
           <cell r="L64">
-            <v>0</v>
+            <v>428.30000000110886</v>
           </cell>
           <cell r="N64">
-            <v>0</v>
+            <v>3572.0000000004106</v>
           </cell>
           <cell r="P64">
             <v>0</v>
@@ -6370,7 +5974,7 @@
             <v>0</v>
           </cell>
           <cell r="T64">
-            <v>0</v>
+            <v>13.880000000001019</v>
           </cell>
           <cell r="V64">
             <v>0</v>
@@ -6380,9 +5984,6 @@
           </cell>
           <cell r="X64">
             <v>0</v>
-          </cell>
-          <cell r="Z64">
-            <v>744</v>
           </cell>
           <cell r="AA64">
             <v>0</v>
@@ -6399,16 +6000,16 @@
             <v>1000</v>
           </cell>
           <cell r="J65">
-            <v>0</v>
+            <v>14873.5</v>
           </cell>
           <cell r="K65">
-            <v>0</v>
+            <v>192.40000000037253</v>
           </cell>
           <cell r="L65">
-            <v>0</v>
+            <v>581.09999999926367</v>
           </cell>
           <cell r="N65">
-            <v>0</v>
+            <v>4318.9999999997372</v>
           </cell>
           <cell r="P65">
             <v>0</v>
@@ -6420,7 +6021,7 @@
             <v>0</v>
           </cell>
           <cell r="T65">
-            <v>0</v>
+            <v>16.389999999999418</v>
           </cell>
           <cell r="V65">
             <v>0</v>
@@ -6430,9 +6031,6 @@
           </cell>
           <cell r="X65">
             <v>0</v>
-          </cell>
-          <cell r="Z65">
-            <v>744</v>
           </cell>
           <cell r="AA65">
             <v>0</v>
@@ -6449,16 +6047,16 @@
             <v>1000</v>
           </cell>
           <cell r="J66">
-            <v>0</v>
+            <v>15683.400000000373</v>
           </cell>
           <cell r="K66">
-            <v>0</v>
+            <v>70.700000001117587</v>
           </cell>
           <cell r="L66">
-            <v>0</v>
+            <v>412.69999999852735</v>
           </cell>
           <cell r="N66">
-            <v>0</v>
+            <v>4434.0000000003211</v>
           </cell>
           <cell r="P66">
             <v>0</v>
@@ -6470,7 +6068,7 @@
             <v>0</v>
           </cell>
           <cell r="T66">
-            <v>0</v>
+            <v>17.069999999999709</v>
           </cell>
           <cell r="V66">
             <v>0</v>
@@ -6480,9 +6078,6 @@
           </cell>
           <cell r="X66">
             <v>0</v>
-          </cell>
-          <cell r="Z66">
-            <v>744</v>
           </cell>
           <cell r="AA66">
             <v>0</v>
@@ -6499,16 +6094,16 @@
             <v>1000</v>
           </cell>
           <cell r="J67">
-            <v>0</v>
+            <v>15453.099999999627</v>
           </cell>
           <cell r="K67">
-            <v>0</v>
+            <v>144.09999999962747</v>
           </cell>
           <cell r="L67">
-            <v>0</v>
+            <v>508.9999999998181</v>
           </cell>
           <cell r="N67">
-            <v>0</v>
+            <v>4373.0000000001828</v>
           </cell>
           <cell r="P67">
             <v>0</v>
@@ -6520,7 +6115,7 @@
             <v>0</v>
           </cell>
           <cell r="T67">
-            <v>0</v>
+            <v>17.090000000000146</v>
           </cell>
           <cell r="V67">
             <v>0</v>
@@ -6530,9 +6125,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>744</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -6584,9 +6176,6 @@
           <cell r="X56">
             <v>0</v>
           </cell>
-          <cell r="Z56">
-            <v>744</v>
-          </cell>
           <cell r="AA56">
             <v>0</v>
           </cell>
@@ -6634,9 +6223,6 @@
           <cell r="X57">
             <v>0</v>
           </cell>
-          <cell r="Z57">
-            <v>744</v>
-          </cell>
           <cell r="AA57">
             <v>0</v>
           </cell>
@@ -6684,9 +6270,6 @@
           <cell r="X58">
             <v>0</v>
           </cell>
-          <cell r="Z58">
-            <v>744</v>
-          </cell>
           <cell r="AA58">
             <v>0</v>
           </cell>
@@ -6732,9 +6315,6 @@
             <v>0</v>
           </cell>
           <cell r="X59">
-            <v>0</v>
-          </cell>
-          <cell r="Z59">
             <v>0</v>
           </cell>
           <cell r="AA59">
@@ -6784,9 +6364,6 @@
           <cell r="X60">
             <v>0</v>
           </cell>
-          <cell r="Z60">
-            <v>744</v>
-          </cell>
           <cell r="AA60">
             <v>0</v>
           </cell>
@@ -6834,9 +6411,6 @@
           <cell r="X61">
             <v>0</v>
           </cell>
-          <cell r="Z61">
-            <v>744</v>
-          </cell>
           <cell r="AA61">
             <v>0</v>
           </cell>
@@ -6846,10 +6420,10 @@
         </row>
         <row r="62">
           <cell r="H62">
-            <v>1330</v>
+            <v>0</v>
           </cell>
           <cell r="I62">
-            <v>1000</v>
+            <v>0</v>
           </cell>
           <cell r="J62">
             <v>0</v>
@@ -6883,9 +6457,6 @@
           </cell>
           <cell r="X62">
             <v>0</v>
-          </cell>
-          <cell r="Z62">
-            <v>744</v>
           </cell>
           <cell r="AA62">
             <v>0</v>
@@ -6896,10 +6467,10 @@
         </row>
         <row r="63">
           <cell r="H63">
-            <v>1330</v>
+            <v>0</v>
           </cell>
           <cell r="I63">
-            <v>1000</v>
+            <v>0</v>
           </cell>
           <cell r="J63">
             <v>0</v>
@@ -6933,9 +6504,6 @@
           </cell>
           <cell r="X63">
             <v>0</v>
-          </cell>
-          <cell r="Z63">
-            <v>744</v>
           </cell>
           <cell r="AA63">
             <v>0</v>
@@ -6946,10 +6514,10 @@
         </row>
         <row r="64">
           <cell r="H64">
-            <v>1330</v>
+            <v>0</v>
           </cell>
           <cell r="I64">
-            <v>1000</v>
+            <v>0</v>
           </cell>
           <cell r="J64">
             <v>0</v>
@@ -6983,9 +6551,6 @@
           </cell>
           <cell r="X64">
             <v>0</v>
-          </cell>
-          <cell r="Z64">
-            <v>744</v>
           </cell>
           <cell r="AA64">
             <v>0</v>
@@ -6996,10 +6561,10 @@
         </row>
         <row r="65">
           <cell r="H65">
-            <v>1330</v>
+            <v>0</v>
           </cell>
           <cell r="I65">
-            <v>1000</v>
+            <v>0</v>
           </cell>
           <cell r="J65">
             <v>0</v>
@@ -7033,9 +6598,6 @@
           </cell>
           <cell r="X65">
             <v>0</v>
-          </cell>
-          <cell r="Z65">
-            <v>744</v>
           </cell>
           <cell r="AA65">
             <v>0</v>
@@ -7046,10 +6608,10 @@
         </row>
         <row r="66">
           <cell r="H66">
-            <v>1330</v>
+            <v>0</v>
           </cell>
           <cell r="I66">
-            <v>1000</v>
+            <v>0</v>
           </cell>
           <cell r="J66">
             <v>0</v>
@@ -7083,9 +6645,6 @@
           </cell>
           <cell r="X66">
             <v>0</v>
-          </cell>
-          <cell r="Z66">
-            <v>744</v>
           </cell>
           <cell r="AA66">
             <v>0</v>
@@ -7096,10 +6655,10 @@
         </row>
         <row r="67">
           <cell r="H67">
-            <v>1330</v>
+            <v>0</v>
           </cell>
           <cell r="I67">
-            <v>1000</v>
+            <v>0</v>
           </cell>
           <cell r="J67">
             <v>0</v>
@@ -7133,9 +6692,6 @@
           </cell>
           <cell r="X67">
             <v>0</v>
-          </cell>
-          <cell r="Z67">
-            <v>744</v>
           </cell>
           <cell r="AA67">
             <v>0</v>
@@ -7453,8 +7009,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3F91E3F4-391D-41D6-A1E8-F5F5CF47988D}">
   <dimension ref="A1:T145"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A139" sqref="A139:A145"/>
+    <sheetView tabSelected="1" topLeftCell="A124" workbookViewId="0">
+      <selection activeCell="G150" sqref="G150"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -7581,8 +7137,8 @@
         <v>12.333333333333336</v>
       </c>
       <c r="N2" s="2">
-        <f>[1]JANUARI!$Z$56</f>
-        <v>744</v>
+        <f>[1]JANUARI!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O2" s="2">
         <f>[1]JANUARI!$V$56</f>
@@ -7660,8 +7216,8 @@
         <v>12.150000000000006</v>
       </c>
       <c r="N3" s="2">
-        <f>[1]JANUARI!$Z$57</f>
-        <v>744</v>
+        <f>[1]JANUARI!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O3" s="2">
         <f>[1]JANUARI!$V$57</f>
@@ -7739,8 +7295,8 @@
         <v>28.616666666666667</v>
       </c>
       <c r="N4" s="2">
-        <f>[1]JANUARI!$Z$58</f>
-        <v>744</v>
+        <f>[1]JANUARI!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O4" s="2">
         <f>[1]JANUARI!$V$58</f>
@@ -7818,8 +7374,8 @@
         <v>0</v>
       </c>
       <c r="N5" s="2">
-        <f>[1]JANUARI!$Z$59</f>
-        <v>744</v>
+        <f>[1]JANUARI!$H$59</f>
+        <v>1000</v>
       </c>
       <c r="O5" s="2">
         <f>[1]JANUARI!$V$59</f>
@@ -7897,8 +7453,8 @@
         <v>43.666666666666679</v>
       </c>
       <c r="N6" s="2">
-        <f>[1]JANUARI!$Z$60</f>
-        <v>744</v>
+        <f>[1]JANUARI!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O6" s="2">
         <f>[1]JANUARI!$V$60</f>
@@ -7976,8 +7532,8 @@
         <v>68.86666666666666</v>
       </c>
       <c r="N7" s="2">
-        <f>[1]JANUARI!$Z$61</f>
-        <v>744</v>
+        <f>[1]JANUARI!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O7" s="2">
         <f>[1]JANUARI!$V$61</f>
@@ -8055,7 +7611,7 @@
         <v>0</v>
       </c>
       <c r="N8" s="2">
-        <f>[1]JANUARI!$Z$62</f>
+        <f>[1]JANUARI!$H$62</f>
         <v>0</v>
       </c>
       <c r="O8" s="2">
@@ -8134,7 +7690,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="2">
-        <f>[1]JANUARI!$Z$63</f>
+        <f>[1]JANUARI!$H$63</f>
         <v>0</v>
       </c>
       <c r="O9" s="2">
@@ -8213,7 +7769,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="2">
-        <f>[1]JANUARI!$Z$64</f>
+        <f>[1]JANUARI!$H$64</f>
         <v>0</v>
       </c>
       <c r="O10" s="2">
@@ -8292,7 +7848,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="2">
-        <f>[1]JANUARI!$Z$65</f>
+        <f>[1]JANUARI!$H$65</f>
         <v>0</v>
       </c>
       <c r="O11" s="2">
@@ -8371,7 +7927,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="2">
-        <f>[1]JANUARI!$Z$66</f>
+        <f>[1]JANUARI!$H$66</f>
         <v>0</v>
       </c>
       <c r="O12" s="2">
@@ -8450,7 +8006,7 @@
         <v>0</v>
       </c>
       <c r="N13" s="2">
-        <f>[1]JANUARI!$Z$67</f>
+        <f>[1]JANUARI!$H$67</f>
         <v>0</v>
       </c>
       <c r="O13" s="2">
@@ -8478,7 +8034,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>2021</v>
       </c>
@@ -8529,8 +8085,8 @@
         <v>3.93333333333333</v>
       </c>
       <c r="N14" s="2">
-        <f>[1]FEBRUARI!$Z$56</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O14" s="2">
         <f>[1]FEBRUARI!$V$56</f>
@@ -8557,7 +8113,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>2021</v>
       </c>
@@ -8608,8 +8164,8 @@
         <v>0.84999999999999964</v>
       </c>
       <c r="N15" s="2">
-        <f>[1]FEBRUARI!$Z$57</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O15" s="2">
         <f>[1]FEBRUARI!$V$57</f>
@@ -8636,7 +8192,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>2021</v>
       </c>
@@ -8687,8 +8243,8 @@
         <v>74.366666666666674</v>
       </c>
       <c r="N16" s="2">
-        <f>[1]FEBRUARI!$Z$58</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O16" s="2">
         <f>[1]FEBRUARI!$V$58</f>
@@ -8715,7 +8271,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>2021</v>
       </c>
@@ -8766,8 +8322,8 @@
         <v>0</v>
       </c>
       <c r="N17" s="2">
-        <f>[1]FEBRUARI!$Z$59</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$59</f>
+        <v>1000</v>
       </c>
       <c r="O17" s="2">
         <f>[1]FEBRUARI!$V$59</f>
@@ -8794,7 +8350,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>2021</v>
       </c>
@@ -8845,8 +8401,8 @@
         <v>133.65333333333334</v>
       </c>
       <c r="N18" s="2">
-        <f>[1]FEBRUARI!$Z$60</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O18" s="2">
         <f>[1]FEBRUARI!$V$60</f>
@@ -8873,7 +8429,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>2021</v>
       </c>
@@ -8924,8 +8480,8 @@
         <v>106.45333333333333</v>
       </c>
       <c r="N19" s="2">
-        <f>[1]FEBRUARI!$Z$61</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O19" s="2">
         <f>[1]FEBRUARI!$V$61</f>
@@ -9003,8 +8559,8 @@
         <v>101.52000000000044</v>
       </c>
       <c r="N20" s="2">
-        <f>[1]FEBRUARI!$Z$62</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O20" s="2">
         <f>[1]FEBRUARI!$V$62</f>
@@ -9082,8 +8638,8 @@
         <v>88.25</v>
       </c>
       <c r="N21" s="2">
-        <f>[1]FEBRUARI!$Z$63</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O21" s="2">
         <f>[1]FEBRUARI!$V$63</f>
@@ -9161,8 +8717,8 @@
         <v>92.349999999998545</v>
       </c>
       <c r="N22" s="2">
-        <f>[1]FEBRUARI!$Z$64</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O22" s="2">
         <f>[1]FEBRUARI!$V$64</f>
@@ -9240,8 +8796,8 @@
         <v>94.989999999999782</v>
       </c>
       <c r="N23" s="2">
-        <f>[1]FEBRUARI!$Z$65</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O23" s="2">
         <f>[1]FEBRUARI!$V$65</f>
@@ -9319,8 +8875,8 @@
         <v>102.35000000000036</v>
       </c>
       <c r="N24" s="2">
-        <f>[1]FEBRUARI!$Z$66</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O24" s="2">
         <f>[1]FEBRUARI!$V$66</f>
@@ -9398,8 +8954,8 @@
         <v>95.159999999999854</v>
       </c>
       <c r="N25" s="2">
-        <f>[1]FEBRUARI!$Z$67</f>
-        <v>672</v>
+        <f>[1]FEBRUARI!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O25" s="2">
         <f>[1]FEBRUARI!$V$67</f>
@@ -9477,8 +9033,8 @@
         <v>0</v>
       </c>
       <c r="N26" s="2">
-        <f>[1]MARET!$Z$56</f>
-        <v>744</v>
+        <f>[1]MARET!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O26" s="2">
         <f>[1]MARET!$V$56</f>
@@ -9556,8 +9112,8 @@
         <v>0</v>
       </c>
       <c r="N27" s="2">
-        <f>[1]MARET!$Z$57</f>
-        <v>744</v>
+        <f>[1]MARET!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O27" s="2">
         <f>[1]MARET!$V$57</f>
@@ -9635,8 +9191,8 @@
         <v>27.066666666666666</v>
       </c>
       <c r="N28" s="2">
-        <f>[1]MARET!$Z$58</f>
-        <v>744</v>
+        <f>[1]MARET!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O28" s="2">
         <f>[1]MARET!$V$58</f>
@@ -9714,8 +9270,8 @@
         <v>0</v>
       </c>
       <c r="N29" s="2">
-        <f>[1]MARET!$Z$59</f>
-        <v>744</v>
+        <f>[1]MARET!$H$59</f>
+        <v>1000</v>
       </c>
       <c r="O29" s="2">
         <f>[1]MARET!$V$59</f>
@@ -9793,8 +9349,8 @@
         <v>57.899999999999991</v>
       </c>
       <c r="N30" s="2">
-        <f>[1]MARET!$Z$60</f>
-        <v>744</v>
+        <f>[1]MARET!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O30" s="2">
         <f>[1]MARET!$V$60</f>
@@ -9872,8 +9428,8 @@
         <v>58.900000000000006</v>
       </c>
       <c r="N31" s="2">
-        <f>[1]MARET!$Z$61</f>
-        <v>744</v>
+        <f>[1]MARET!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O31" s="2">
         <f>[1]MARET!$V$61</f>
@@ -9951,8 +9507,8 @@
         <v>63.429999999998472</v>
       </c>
       <c r="N32" s="2">
-        <f>[1]MARET!$Z$62</f>
-        <v>744</v>
+        <f>[1]MARET!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O32" s="2">
         <f>[1]MARET!$V$62</f>
@@ -10030,8 +9586,8 @@
         <v>71.069999999999709</v>
       </c>
       <c r="N33" s="2">
-        <f>[1]MARET!$Z$63</f>
-        <v>744</v>
+        <f>[1]MARET!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O33" s="2">
         <f>[1]MARET!$V$63</f>
@@ -10109,8 +9665,8 @@
         <v>65.079999999999927</v>
       </c>
       <c r="N34" s="2">
-        <f>[1]MARET!$Z$64</f>
-        <v>744</v>
+        <f>[1]MARET!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O34" s="2">
         <f>[1]MARET!$V$64</f>
@@ -10188,8 +9744,8 @@
         <v>65.059999999999491</v>
       </c>
       <c r="N35" s="2">
-        <f>[1]MARET!$Z$65</f>
-        <v>744</v>
+        <f>[1]MARET!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O35" s="2">
         <f>[1]MARET!$V$65</f>
@@ -10267,8 +9823,8 @@
         <v>58.809999999999491</v>
       </c>
       <c r="N36" s="2">
-        <f>[1]MARET!$Z$66</f>
-        <v>744</v>
+        <f>[1]MARET!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O36" s="2">
         <f>[1]MARET!$V$66</f>
@@ -10346,8 +9902,8 @@
         <v>58.659999999999854</v>
       </c>
       <c r="N37" s="2">
-        <f>[1]MARET!$Z$67</f>
-        <v>744</v>
+        <f>[1]MARET!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O37" s="2">
         <f>[1]MARET!$V$67</f>
@@ -10374,7 +9930,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A38">
         <v>2021</v>
       </c>
@@ -10425,8 +9981,8 @@
         <v>12.866666666666664</v>
       </c>
       <c r="N38" s="2">
-        <f>[1]APRIL!$Z$56</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O38" s="2">
         <f>[1]APRIL!$V$56</f>
@@ -10453,7 +10009,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A39">
         <v>2021</v>
       </c>
@@ -10504,8 +10060,8 @@
         <v>3.4</v>
       </c>
       <c r="N39" s="2">
-        <f>[1]APRIL!$Z$57</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O39" s="2">
         <f>[1]APRIL!$V$57</f>
@@ -10532,7 +10088,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A40">
         <v>2021</v>
       </c>
@@ -10583,8 +10139,8 @@
         <v>26.68333333333333</v>
       </c>
       <c r="N40" s="2">
-        <f>[1]APRIL!$Z$58</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O40" s="2">
         <f>[1]APRIL!$V$58</f>
@@ -10611,7 +10167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A41">
         <v>2021</v>
       </c>
@@ -10662,8 +10218,8 @@
         <v>0</v>
       </c>
       <c r="N41" s="2">
-        <f>[1]APRIL!$Z$59</f>
-        <v>0</v>
+        <f>[1]APRIL!$H$59</f>
+        <v>1000</v>
       </c>
       <c r="O41" s="2">
         <f>[1]APRIL!$V$59</f>
@@ -10690,7 +10246,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A42">
         <v>2021</v>
       </c>
@@ -10741,8 +10297,8 @@
         <v>106.28333333333333</v>
       </c>
       <c r="N42" s="2">
-        <f>[1]APRIL!$Z$60</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O42" s="2">
         <f>[1]APRIL!$V$60</f>
@@ -10769,7 +10325,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A43">
         <v>2021</v>
       </c>
@@ -10820,8 +10376,8 @@
         <v>87.466666666666669</v>
       </c>
       <c r="N43" s="2">
-        <f>[1]APRIL!$Z$61</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O43" s="2">
         <f>[1]APRIL!$V$61</f>
@@ -10899,8 +10455,8 @@
         <v>153.80000000000109</v>
       </c>
       <c r="N44" s="2">
-        <f>[1]APRIL!$Z$62</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O44" s="2">
         <f>[1]APRIL!$V$62</f>
@@ -10978,8 +10534,8 @@
         <v>141.5</v>
       </c>
       <c r="N45" s="2">
-        <f>[1]APRIL!$Z$63</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O45" s="2">
         <f>[1]APRIL!$V$63</f>
@@ -11057,8 +10613,8 @@
         <v>178.36000000000058</v>
       </c>
       <c r="N46" s="2">
-        <f>[1]APRIL!$Z$64</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O46" s="2">
         <f>[1]APRIL!$V$64</f>
@@ -11136,8 +10692,8 @@
         <v>183.86000000000058</v>
       </c>
       <c r="N47" s="2">
-        <f>[1]APRIL!$Z$65</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O47" s="2">
         <f>[1]APRIL!$V$65</f>
@@ -11215,8 +10771,8 @@
         <v>185.06000000000131</v>
       </c>
       <c r="N48" s="2">
-        <f>[1]APRIL!$Z$66</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O48" s="2">
         <f>[1]APRIL!$V$66</f>
@@ -11294,8 +10850,8 @@
         <v>159.3700000000008</v>
       </c>
       <c r="N49" s="2">
-        <f>[1]APRIL!$Z$67</f>
-        <v>720</v>
+        <f>[1]APRIL!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O49" s="2">
         <f>[1]APRIL!$V$67</f>
@@ -11373,8 +10929,8 @@
         <v>0</v>
       </c>
       <c r="N50" s="2">
-        <f>[1]MEI!$Z$56</f>
-        <v>744</v>
+        <f>[1]MEI!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O50" s="2">
         <f>[1]MEI!$V$56</f>
@@ -11452,8 +11008,8 @@
         <v>0</v>
       </c>
       <c r="N51" s="2">
-        <f>[1]MEI!$Z$57</f>
-        <v>744</v>
+        <f>[1]MEI!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O51" s="2">
         <f>[1]MEI!$V$57</f>
@@ -11531,8 +11087,8 @@
         <v>5.7000000000000028</v>
       </c>
       <c r="N52" s="2">
-        <f>[1]MEI!$Z$58</f>
-        <v>744</v>
+        <f>[1]MEI!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O52" s="2">
         <f>[1]MEI!$V$58</f>
@@ -11610,8 +11166,8 @@
         <v>0</v>
       </c>
       <c r="N53" s="2">
-        <f>[1]MEI!$Z$59</f>
-        <v>0</v>
+        <f>[1]MEI!$H$59</f>
+        <v>1000</v>
       </c>
       <c r="O53" s="2">
         <f>[1]MEI!$V$59</f>
@@ -11689,8 +11245,8 @@
         <v>224.76666666666671</v>
       </c>
       <c r="N54" s="2">
-        <f>[1]MEI!$Z$60</f>
-        <v>744</v>
+        <f>[1]MEI!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O54" s="2">
         <f>[1]MEI!$V$60</f>
@@ -11768,8 +11324,8 @@
         <v>180.08333333333331</v>
       </c>
       <c r="N55" s="2">
-        <f>[1]MEI!$Z$61</f>
-        <v>744</v>
+        <f>[1]MEI!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O55" s="2">
         <f>[1]MEI!$V$61</f>
@@ -11847,8 +11403,8 @@
         <v>302.18000000000029</v>
       </c>
       <c r="N56" s="2">
-        <f>[1]MEI!$Z$62</f>
-        <v>744</v>
+        <f>[1]MEI!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O56" s="2">
         <f>[1]MEI!$V$62</f>
@@ -11926,8 +11482,8 @@
         <v>173.44000000000051</v>
       </c>
       <c r="N57" s="2">
-        <f>[1]MEI!$Z$63</f>
-        <v>744</v>
+        <f>[1]MEI!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O57" s="2">
         <f>[1]MEI!$V$63</f>
@@ -12005,8 +11561,8 @@
         <v>310.78000000000065</v>
       </c>
       <c r="N58" s="2">
-        <f>[1]MEI!$Z$64</f>
-        <v>744</v>
+        <f>[1]MEI!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O58" s="2">
         <f>[1]MEI!$V$64</f>
@@ -12084,8 +11640,8 @@
         <v>310.1299999999992</v>
       </c>
       <c r="N59" s="2">
-        <f>[1]MEI!$Z$65</f>
-        <v>744</v>
+        <f>[1]MEI!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O59" s="2">
         <f>[1]MEI!$V$65</f>
@@ -12163,8 +11719,8 @@
         <v>327.65999999999985</v>
       </c>
       <c r="N60" s="2">
-        <f>[1]MEI!$Z$66</f>
-        <v>744</v>
+        <f>[1]MEI!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O60" s="2">
         <f>[1]MEI!$V$66</f>
@@ -12242,8 +11798,8 @@
         <v>319.46999999999935</v>
       </c>
       <c r="N61" s="2">
-        <f>[1]MEI!$Z$67</f>
-        <v>744</v>
+        <f>[1]MEI!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O61" s="2">
         <f>[1]MEI!$V$67</f>
@@ -12270,7 +11826,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="62" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A62">
         <v>2021</v>
       </c>
@@ -12321,8 +11877,8 @@
         <v>0</v>
       </c>
       <c r="N62" s="2">
-        <f>[1]JUNI!$Z$56</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O62" s="2">
         <f>[1]JUNI!$V$56</f>
@@ -12349,7 +11905,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="63" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A63">
         <v>2021</v>
       </c>
@@ -12400,8 +11956,8 @@
         <v>0</v>
       </c>
       <c r="N63" s="2">
-        <f>[1]JUNI!$Z$57</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O63" s="2">
         <f>[1]JUNI!$V$57</f>
@@ -12428,7 +11984,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="64" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A64">
         <v>2021</v>
       </c>
@@ -12479,8 +12035,8 @@
         <v>36.200000000000003</v>
       </c>
       <c r="N64" s="2">
-        <f>[1]JUNI!$Z$58</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O64" s="2">
         <f>[1]JUNI!$V$58</f>
@@ -12507,7 +12063,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="65" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A65">
         <v>2021</v>
       </c>
@@ -12558,7 +12114,7 @@
         <v>0</v>
       </c>
       <c r="N65" s="2">
-        <f>[1]JUNI!$Z$59</f>
+        <f>[1]JUNI!$H$59</f>
         <v>0</v>
       </c>
       <c r="O65" s="2">
@@ -12586,7 +12142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="66" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A66">
         <v>2021</v>
       </c>
@@ -12637,8 +12193,8 @@
         <v>101.26666666666667</v>
       </c>
       <c r="N66" s="2">
-        <f>[1]JUNI!$Z$60</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O66" s="2">
         <f>[1]JUNI!$V$60</f>
@@ -12665,7 +12221,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="67" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A67">
         <v>2021</v>
       </c>
@@ -12716,8 +12272,8 @@
         <v>83.59999999999998</v>
       </c>
       <c r="N67" s="2">
-        <f>[1]JUNI!$Z$61</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O67" s="2">
         <f>[1]JUNI!$V$61</f>
@@ -12795,8 +12351,8 @@
         <v>129.84000000000015</v>
       </c>
       <c r="N68" s="2">
-        <f>[1]JUNI!$Z$62</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O68" s="2">
         <f>[1]JUNI!$V$62</f>
@@ -12874,8 +12430,8 @@
         <v>25.909999999999854</v>
       </c>
       <c r="N69" s="2">
-        <f>[1]JUNI!$Z$63</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O69" s="2">
         <f>[1]JUNI!$V$63</f>
@@ -12953,8 +12509,8 @@
         <v>125.73999999999978</v>
       </c>
       <c r="N70" s="2">
-        <f>[1]JUNI!$Z$64</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O70" s="2">
         <f>[1]JUNI!$V$64</f>
@@ -13032,8 +12588,8 @@
         <v>133.96000000000095</v>
       </c>
       <c r="N71" s="2">
-        <f>[1]JUNI!$Z$65</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O71" s="2">
         <f>[1]JUNI!$V$65</f>
@@ -13111,8 +12667,8 @@
         <v>124.15999999999985</v>
       </c>
       <c r="N72" s="2">
-        <f>[1]JUNI!$Z$66</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O72" s="2">
         <f>[1]JUNI!$V$66</f>
@@ -13190,8 +12746,8 @@
         <v>135.23999999999978</v>
       </c>
       <c r="N73" s="2">
-        <f>[1]JUNI!$Z$67</f>
-        <v>720</v>
+        <f>[1]JUNI!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O73" s="2">
         <f>[1]JUNI!$V$67</f>
@@ -13269,8 +12825,8 @@
         <v>0</v>
       </c>
       <c r="N74" s="2">
-        <f>[1]JULI!$Z$56</f>
-        <v>744</v>
+        <f>[1]JULI!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O74" s="2">
         <f>[1]JULI!$V$56</f>
@@ -13348,8 +12904,8 @@
         <v>0</v>
       </c>
       <c r="N75" s="2">
-        <f>[1]JULI!$Z$57</f>
-        <v>744</v>
+        <f>[1]JULI!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O75" s="2">
         <f>[1]JULI!$V$57</f>
@@ -13427,8 +12983,8 @@
         <v>0</v>
       </c>
       <c r="N76" s="2">
-        <f>[1]JULI!$Z$58</f>
-        <v>744</v>
+        <f>[1]JULI!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O76" s="2">
         <f>[1]JULI!$V$58</f>
@@ -13506,7 +13062,7 @@
         <v>0</v>
       </c>
       <c r="N77" s="2">
-        <f>[1]JULI!$Z$59</f>
+        <f>[1]JULI!$H$59</f>
         <v>0</v>
       </c>
       <c r="O77" s="2">
@@ -13585,8 +13141,8 @@
         <v>36.18333333333333</v>
       </c>
       <c r="N78" s="2">
-        <f>[1]JULI!$Z$60</f>
-        <v>744</v>
+        <f>[1]JULI!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O78" s="2">
         <f>[1]JULI!$V$60</f>
@@ -13664,8 +13220,8 @@
         <v>34.949999999999989</v>
       </c>
       <c r="N79" s="2">
-        <f>[1]JULI!$Z$61</f>
-        <v>744</v>
+        <f>[1]JULI!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O79" s="2">
         <f>[1]JULI!$V$61</f>
@@ -13743,8 +13299,8 @@
         <v>39.649999999999636</v>
       </c>
       <c r="N80" s="2">
-        <f>[1]JULI!$Z$62</f>
-        <v>744</v>
+        <f>[1]JULI!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O80" s="2">
         <f>[1]JULI!$V$62</f>
@@ -13822,8 +13378,8 @@
         <v>47.049999999999272</v>
       </c>
       <c r="N81" s="2">
-        <f>[1]JULI!$Z$63</f>
-        <v>744</v>
+        <f>[1]JULI!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O81" s="2">
         <f>[1]JULI!$V$63</f>
@@ -13901,8 +13457,8 @@
         <v>40.159999999999854</v>
       </c>
       <c r="N82" s="2">
-        <f>[1]JULI!$Z$64</f>
-        <v>744</v>
+        <f>[1]JULI!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O82" s="2">
         <f>[1]JULI!$V$64</f>
@@ -13980,8 +13536,8 @@
         <v>43.969999999999345</v>
       </c>
       <c r="N83" s="2">
-        <f>[1]JULI!$Z$65</f>
-        <v>744</v>
+        <f>[1]JULI!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O83" s="2">
         <f>[1]JULI!$V$65</f>
@@ -14059,8 +13615,8 @@
         <v>52.049999999999272</v>
       </c>
       <c r="N84" s="2">
-        <f>[1]JULI!$Z$66</f>
-        <v>744</v>
+        <f>[1]JULI!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O84" s="2">
         <f>[1]JULI!$V$66</f>
@@ -14138,8 +13694,8 @@
         <v>48.909999999999854</v>
       </c>
       <c r="N85" s="2">
-        <f>[1]JULI!$Z$67</f>
-        <v>744</v>
+        <f>[1]JULI!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O85" s="2">
         <f>[1]JULI!$V$67</f>
@@ -14166,7 +13722,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="86" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A86">
         <v>2021</v>
       </c>
@@ -14217,8 +13773,8 @@
         <v>0</v>
       </c>
       <c r="N86" s="2">
-        <f>[1]AGUSTUS!$Z$56</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O86" s="2">
         <f>[1]AGUSTUS!$V$56</f>
@@ -14245,7 +13801,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="87" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A87">
         <v>2021</v>
       </c>
@@ -14296,8 +13852,8 @@
         <v>0</v>
       </c>
       <c r="N87" s="2">
-        <f>[1]AGUSTUS!$Z$57</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O87" s="2">
         <f>[1]AGUSTUS!$V$57</f>
@@ -14324,7 +13880,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="88" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A88">
         <v>2021</v>
       </c>
@@ -14375,8 +13931,8 @@
         <v>0</v>
       </c>
       <c r="N88" s="2">
-        <f>[1]AGUSTUS!$Z$58</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O88" s="2">
         <f>[1]AGUSTUS!$V$58</f>
@@ -14403,7 +13959,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="89" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A89">
         <v>2021</v>
       </c>
@@ -14454,7 +14010,7 @@
         <v>0</v>
       </c>
       <c r="N89" s="2">
-        <f>[1]AGUSTUS!$Z$59</f>
+        <f>[1]AGUSTUS!$H$59</f>
         <v>0</v>
       </c>
       <c r="O89" s="2">
@@ -14482,7 +14038,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="90" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A90">
         <v>2021</v>
       </c>
@@ -14533,8 +14089,8 @@
         <v>26.5</v>
       </c>
       <c r="N90" s="2">
-        <f>[1]AGUSTUS!$Z$60</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O90" s="2">
         <f>[1]AGUSTUS!$V$60</f>
@@ -14561,7 +14117,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="91" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A91">
         <v>2021</v>
       </c>
@@ -14612,8 +14168,8 @@
         <v>24.349999999999998</v>
       </c>
       <c r="N91" s="2">
-        <f>[1]AGUSTUS!$Z$61</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O91" s="2">
         <f>[1]AGUSTUS!$V$61</f>
@@ -14691,8 +14247,8 @@
         <v>19.520000000000437</v>
       </c>
       <c r="N92" s="2">
-        <f>[1]AGUSTUS!$Z$62</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O92" s="2">
         <f>[1]AGUSTUS!$V$62</f>
@@ -14770,8 +14326,8 @@
         <v>18.030000000000655</v>
       </c>
       <c r="N93" s="2">
-        <f>[1]AGUSTUS!$Z$63</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O93" s="2">
         <f>[1]AGUSTUS!$V$63</f>
@@ -14849,8 +14405,8 @@
         <v>14.319999999999709</v>
       </c>
       <c r="N94" s="2">
-        <f>[1]AGUSTUS!$Z$64</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O94" s="2">
         <f>[1]AGUSTUS!$V$64</f>
@@ -14928,8 +14484,8 @@
         <v>21.180000000000291</v>
       </c>
       <c r="N95" s="2">
-        <f>[1]AGUSTUS!$Z$65</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O95" s="2">
         <f>[1]AGUSTUS!$V$65</f>
@@ -15007,8 +14563,8 @@
         <v>22.819999999999709</v>
       </c>
       <c r="N96" s="2">
-        <f>[1]AGUSTUS!$Z$66</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O96" s="2">
         <f>[1]AGUSTUS!$V$66</f>
@@ -15086,8 +14642,8 @@
         <v>23.069999999999709</v>
       </c>
       <c r="N97" s="2">
-        <f>[1]AGUSTUS!$Z$67</f>
-        <v>744</v>
+        <f>[1]AGUSTUS!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O97" s="2">
         <f>[1]AGUSTUS!$V$67</f>
@@ -15165,8 +14721,8 @@
         <v>0</v>
       </c>
       <c r="N98" s="2">
-        <f>[1]SEPTEMBER!$Z$56</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O98" s="2">
         <f>[1]SEPTEMBER!$V$56</f>
@@ -15244,8 +14800,8 @@
         <v>0</v>
       </c>
       <c r="N99" s="2">
-        <f>[1]SEPTEMBER!$Z$57</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O99" s="2">
         <f>[1]SEPTEMBER!$V$57</f>
@@ -15323,8 +14879,8 @@
         <v>0</v>
       </c>
       <c r="N100" s="2">
-        <f>[1]SEPTEMBER!$Z$58</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O100" s="2">
         <f>[1]SEPTEMBER!$V$58</f>
@@ -15402,7 +14958,7 @@
         <v>0</v>
       </c>
       <c r="N101" s="2">
-        <f>[1]SEPTEMBER!$Z$59</f>
+        <f>[1]SEPTEMBER!$H$59</f>
         <v>0</v>
       </c>
       <c r="O101" s="2">
@@ -15481,8 +15037,8 @@
         <v>5.6833333333333291</v>
       </c>
       <c r="N102" s="2">
-        <f>[1]SEPTEMBER!$Z$60</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O102" s="2">
         <f>[1]SEPTEMBER!$V$60</f>
@@ -15560,8 +15116,8 @@
         <v>4.4833333333333361</v>
       </c>
       <c r="N103" s="2">
-        <f>[1]SEPTEMBER!$Z$61</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O103" s="2">
         <f>[1]SEPTEMBER!$V$61</f>
@@ -15639,8 +15195,8 @@
         <v>4.9399999999986903</v>
       </c>
       <c r="N104" s="2">
-        <f>[1]SEPTEMBER!$Z$62</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O104" s="2">
         <f>[1]SEPTEMBER!$V$62</f>
@@ -15718,8 +15274,8 @@
         <v>8.0299999999988358</v>
       </c>
       <c r="N105" s="2">
-        <f>[1]SEPTEMBER!$Z$63</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O105" s="2">
         <f>[1]SEPTEMBER!$V$63</f>
@@ -15797,8 +15353,8 @@
         <v>6.7700000000004366</v>
       </c>
       <c r="N106" s="2">
-        <f>[1]SEPTEMBER!$Z$64</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O106" s="2">
         <f>[1]SEPTEMBER!$V$64</f>
@@ -15876,8 +15432,8 @@
         <v>7.930000000000291</v>
       </c>
       <c r="N107" s="2">
-        <f>[1]SEPTEMBER!$Z$65</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O107" s="2">
         <f>[1]SEPTEMBER!$V$65</f>
@@ -15955,8 +15511,8 @@
         <v>8.0200000000004366</v>
       </c>
       <c r="N108" s="2">
-        <f>[1]SEPTEMBER!$Z$66</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O108" s="2">
         <f>[1]SEPTEMBER!$V$66</f>
@@ -16034,8 +15590,8 @@
         <v>8.0300000000006548</v>
       </c>
       <c r="N109" s="2">
-        <f>[1]SEPTEMBER!$Z$67</f>
-        <v>720</v>
+        <f>[1]SEPTEMBER!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O109" s="2">
         <f>[1]SEPTEMBER!$V$67</f>
@@ -16062,7 +15618,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="110" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A110">
         <v>2021</v>
       </c>
@@ -16113,8 +15669,8 @@
         <v>0</v>
       </c>
       <c r="N110" s="2">
-        <f>[1]OKTOBER!$Z$56</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O110" s="2">
         <f>[1]OKTOBER!$V$56</f>
@@ -16141,7 +15697,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="111" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A111">
         <v>2021</v>
       </c>
@@ -16192,8 +15748,8 @@
         <v>0</v>
       </c>
       <c r="N111" s="2">
-        <f>[1]OKTOBER!$Z$57</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O111" s="2">
         <f>[1]OKTOBER!$V$57</f>
@@ -16220,7 +15776,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="112" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A112">
         <v>2021</v>
       </c>
@@ -16271,8 +15827,8 @@
         <v>0</v>
       </c>
       <c r="N112" s="2">
-        <f>[1]OKTOBER!$Z$58</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O112" s="2">
         <f>[1]OKTOBER!$V$58</f>
@@ -16299,7 +15855,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="113" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A113">
         <v>2021</v>
       </c>
@@ -16350,7 +15906,7 @@
         <v>0</v>
       </c>
       <c r="N113" s="2">
-        <f>[1]OKTOBER!$Z$59</f>
+        <f>[1]OKTOBER!$H$59</f>
         <v>0</v>
       </c>
       <c r="O113" s="2">
@@ -16378,7 +15934,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="114" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A114">
         <v>2021</v>
       </c>
@@ -16429,8 +15985,8 @@
         <v>20.43333333333333</v>
       </c>
       <c r="N114" s="2">
-        <f>[1]OKTOBER!$Z$60</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O114" s="2">
         <f>[1]OKTOBER!$V$60</f>
@@ -16457,7 +16013,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="115" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>2021</v>
       </c>
@@ -16508,8 +16064,8 @@
         <v>20.250000000000004</v>
       </c>
       <c r="N115" s="2">
-        <f>[1]OKTOBER!$Z$61</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O115" s="2">
         <f>[1]OKTOBER!$V$61</f>
@@ -16587,8 +16143,8 @@
         <v>10.540000000000873</v>
       </c>
       <c r="N116" s="2">
-        <f>[1]OKTOBER!$Z$62</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O116" s="2">
         <f>[1]OKTOBER!$V$62</f>
@@ -16666,8 +16222,8 @@
         <v>12.6200000000008</v>
       </c>
       <c r="N117" s="2">
-        <f>[1]OKTOBER!$Z$63</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O117" s="2">
         <f>[1]OKTOBER!$V$63</f>
@@ -16745,8 +16301,8 @@
         <v>12.869999999998981</v>
       </c>
       <c r="N118" s="2">
-        <f>[1]OKTOBER!$Z$64</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O118" s="2">
         <f>[1]OKTOBER!$V$64</f>
@@ -16824,8 +16380,8 @@
         <v>14.690000000000509</v>
       </c>
       <c r="N119" s="2">
-        <f>[1]OKTOBER!$Z$65</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O119" s="2">
         <f>[1]OKTOBER!$V$65</f>
@@ -16903,8 +16459,8 @@
         <v>16.159999999999854</v>
       </c>
       <c r="N120" s="2">
-        <f>[1]OKTOBER!$Z$66</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O120" s="2">
         <f>[1]OKTOBER!$V$66</f>
@@ -16982,8 +16538,8 @@
         <v>14.899999999999636</v>
       </c>
       <c r="N121" s="2">
-        <f>[1]OKTOBER!$Z$67</f>
-        <v>744</v>
+        <f>[1]OKTOBER!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O121" s="2">
         <f>[1]OKTOBER!$V$67</f>
@@ -17030,19 +16586,19 @@
       </c>
       <c r="F122" s="2">
         <f>[1]NOVEMBER!$J$56</f>
-        <v>0</v>
+        <v>220</v>
       </c>
       <c r="G122" s="2">
         <f>[1]NOVEMBER!$K$56</f>
-        <v>0</v>
+        <v>9.0000000000009095</v>
       </c>
       <c r="H122" s="2">
         <f>[1]NOVEMBER!$L$56</f>
-        <v>0</v>
+        <v>3.52</v>
       </c>
       <c r="I122" s="2">
         <f>[1]NOVEMBER!$N$56</f>
-        <v>0</v>
+        <v>116</v>
       </c>
       <c r="J122" s="2">
         <f>[1]NOVEMBER!$P$56</f>
@@ -17058,11 +16614,11 @@
       </c>
       <c r="M122" s="2">
         <f>[1]NOVEMBER!$T$56</f>
-        <v>0</v>
+        <v>1.1000000000000014</v>
       </c>
       <c r="N122" s="2">
-        <f>[1]NOVEMBER!$Z$56</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O122" s="2">
         <f>[1]NOVEMBER!$V$56</f>
@@ -17109,19 +16665,19 @@
       </c>
       <c r="F123" s="2">
         <f>[1]NOVEMBER!$J$57</f>
-        <v>0</v>
+        <v>3330</v>
       </c>
       <c r="G123" s="2">
         <f>[1]NOVEMBER!$K$57</f>
-        <v>0</v>
+        <v>224</v>
       </c>
       <c r="H123" s="2">
         <f>[1]NOVEMBER!$L$57</f>
-        <v>0</v>
+        <v>53.28</v>
       </c>
       <c r="I123" s="2">
         <f>[1]NOVEMBER!$N$57</f>
-        <v>0</v>
+        <v>1286</v>
       </c>
       <c r="J123" s="2">
         <f>[1]NOVEMBER!$P$57</f>
@@ -17137,11 +16693,11 @@
       </c>
       <c r="M123" s="2">
         <f>[1]NOVEMBER!$T$57</f>
-        <v>0</v>
+        <v>14.666666666666664</v>
       </c>
       <c r="N123" s="2">
-        <f>[1]NOVEMBER!$Z$57</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O123" s="2">
         <f>[1]NOVEMBER!$V$57</f>
@@ -17192,7 +16748,7 @@
       </c>
       <c r="G124" s="2">
         <f>[1]NOVEMBER!$K$58</f>
-        <v>0</v>
+        <v>7.9999999998835847</v>
       </c>
       <c r="H124" s="2">
         <f>[1]NOVEMBER!$L$58</f>
@@ -17219,8 +16775,8 @@
         <v>0</v>
       </c>
       <c r="N124" s="2">
-        <f>[1]NOVEMBER!$Z$58</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O124" s="2">
         <f>[1]NOVEMBER!$V$58</f>
@@ -17298,7 +16854,7 @@
         <v>0</v>
       </c>
       <c r="N125" s="2">
-        <f>[1]NOVEMBER!$Z$59</f>
+        <f>[1]NOVEMBER!$H$59</f>
         <v>0</v>
       </c>
       <c r="O125" s="2">
@@ -17346,19 +16902,19 @@
       </c>
       <c r="F126" s="2">
         <f>[1]NOVEMBER!$J$60</f>
-        <v>34370</v>
+        <v>31950</v>
       </c>
       <c r="G126" s="2">
         <f>[1]NOVEMBER!$K$60</f>
-        <v>1026</v>
+        <v>970</v>
       </c>
       <c r="H126" s="2">
         <f>[1]NOVEMBER!$L$60</f>
-        <v>549.91999999999996</v>
+        <v>511.2</v>
       </c>
       <c r="I126" s="2">
         <f>[1]NOVEMBER!$N$60</f>
-        <v>9511</v>
+        <v>8825</v>
       </c>
       <c r="J126" s="2">
         <f>[1]NOVEMBER!$P$60</f>
@@ -17374,11 +16930,11 @@
       </c>
       <c r="M126" s="2">
         <f>[1]NOVEMBER!$T$60</f>
-        <v>22.383333333333329</v>
+        <v>21.483333333333345</v>
       </c>
       <c r="N126" s="2">
-        <f>[1]NOVEMBER!$Z$60</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O126" s="2">
         <f>[1]NOVEMBER!$V$60</f>
@@ -17425,19 +16981,19 @@
       </c>
       <c r="F127" s="2">
         <f>[1]NOVEMBER!$J$61</f>
-        <v>31150</v>
+        <v>25240</v>
       </c>
       <c r="G127" s="2">
         <f>[1]NOVEMBER!$K$61</f>
-        <v>1046</v>
+        <v>902</v>
       </c>
       <c r="H127" s="2">
         <f>[1]NOVEMBER!$L$61</f>
-        <v>498.40000000000003</v>
+        <v>403.84000000000003</v>
       </c>
       <c r="I127" s="2">
         <f>[1]NOVEMBER!$N$61</f>
-        <v>8363</v>
+        <v>6926</v>
       </c>
       <c r="J127" s="2">
         <f>[1]NOVEMBER!$P$61</f>
@@ -17453,11 +17009,11 @@
       </c>
       <c r="M127" s="2">
         <f>[1]NOVEMBER!$T$61</f>
-        <v>21.79999999999999</v>
+        <v>18.733333333333334</v>
       </c>
       <c r="N127" s="2">
-        <f>[1]NOVEMBER!$Z$61</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O127" s="2">
         <f>[1]NOVEMBER!$V$61</f>
@@ -17504,19 +17060,19 @@
       </c>
       <c r="F128" s="2">
         <f>[1]NOVEMBER!$J$62</f>
-        <v>0</v>
+        <v>10802.599999999627</v>
       </c>
       <c r="G128" s="2">
         <f>[1]NOVEMBER!$K$62</f>
-        <v>0</v>
+        <v>58.900000000372529</v>
       </c>
       <c r="H128" s="2">
         <f>[1]NOVEMBER!$L$62</f>
-        <v>0</v>
+        <v>243.69999999925494</v>
       </c>
       <c r="I128" s="2">
         <f>[1]NOVEMBER!$N$62</f>
-        <v>0</v>
+        <v>3103.0000000000459</v>
       </c>
       <c r="J128" s="2">
         <f>[1]NOVEMBER!$P$62</f>
@@ -17532,11 +17088,11 @@
       </c>
       <c r="M128" s="2">
         <f>[1]NOVEMBER!$T$62</f>
-        <v>0</v>
+        <v>12.049999999999272</v>
       </c>
       <c r="N128" s="2">
-        <f>[1]NOVEMBER!$Z$62</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$62</f>
+        <v>1330</v>
       </c>
       <c r="O128" s="2">
         <f>[1]NOVEMBER!$V$62</f>
@@ -17583,19 +17139,19 @@
       </c>
       <c r="F129" s="2">
         <f>[1]NOVEMBER!$J$63</f>
-        <v>0</v>
+        <v>11934.400000000373</v>
       </c>
       <c r="G129" s="2">
         <f>[1]NOVEMBER!$K$63</f>
-        <v>0</v>
+        <v>138.19999999925494</v>
       </c>
       <c r="H129" s="2">
         <f>[1]NOVEMBER!$L$63</f>
-        <v>0</v>
+        <v>496.20000000184518</v>
       </c>
       <c r="I129" s="2">
         <f>[1]NOVEMBER!$N$63</f>
-        <v>0</v>
+        <v>3467.000000000517</v>
       </c>
       <c r="J129" s="2">
         <f>[1]NOVEMBER!$P$63</f>
@@ -17611,11 +17167,11 @@
       </c>
       <c r="M129" s="2">
         <f>[1]NOVEMBER!$T$63</f>
-        <v>0</v>
+        <v>13.329999999999927</v>
       </c>
       <c r="N129" s="2">
-        <f>[1]NOVEMBER!$Z$63</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$63</f>
+        <v>1330</v>
       </c>
       <c r="O129" s="2">
         <f>[1]NOVEMBER!$V$63</f>
@@ -17662,19 +17218,19 @@
       </c>
       <c r="F130" s="2">
         <f>[1]NOVEMBER!$J$64</f>
-        <v>0</v>
+        <v>12485.599999999627</v>
       </c>
       <c r="G130" s="2">
         <f>[1]NOVEMBER!$K$64</f>
-        <v>0</v>
+        <v>157.29999999888241</v>
       </c>
       <c r="H130" s="2">
         <f>[1]NOVEMBER!$L$64</f>
-        <v>0</v>
+        <v>428.30000000110886</v>
       </c>
       <c r="I130" s="2">
         <f>[1]NOVEMBER!$N$64</f>
-        <v>0</v>
+        <v>3572.0000000004106</v>
       </c>
       <c r="J130" s="2">
         <f>[1]NOVEMBER!$P$64</f>
@@ -17690,11 +17246,11 @@
       </c>
       <c r="M130" s="2">
         <f>[1]NOVEMBER!$T$64</f>
-        <v>0</v>
+        <v>13.880000000001019</v>
       </c>
       <c r="N130" s="2">
-        <f>[1]NOVEMBER!$Z$64</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$64</f>
+        <v>1330</v>
       </c>
       <c r="O130" s="2">
         <f>[1]NOVEMBER!$V$64</f>
@@ -17741,19 +17297,19 @@
       </c>
       <c r="F131" s="2">
         <f>[1]NOVEMBER!$J$65</f>
-        <v>0</v>
+        <v>14873.5</v>
       </c>
       <c r="G131" s="2">
         <f>[1]NOVEMBER!$K$65</f>
-        <v>0</v>
+        <v>192.40000000037253</v>
       </c>
       <c r="H131" s="2">
         <f>[1]NOVEMBER!$L$65</f>
-        <v>0</v>
+        <v>581.09999999926367</v>
       </c>
       <c r="I131" s="2">
         <f>[1]NOVEMBER!$N$65</f>
-        <v>0</v>
+        <v>4318.9999999997372</v>
       </c>
       <c r="J131" s="2">
         <f>[1]NOVEMBER!$P$65</f>
@@ -17769,11 +17325,11 @@
       </c>
       <c r="M131" s="2">
         <f>[1]NOVEMBER!$T$65</f>
-        <v>0</v>
+        <v>16.389999999999418</v>
       </c>
       <c r="N131" s="2">
-        <f>[1]NOVEMBER!$Z$65</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$65</f>
+        <v>1330</v>
       </c>
       <c r="O131" s="2">
         <f>[1]NOVEMBER!$V$65</f>
@@ -17820,19 +17376,19 @@
       </c>
       <c r="F132" s="2">
         <f>[1]NOVEMBER!$J$66</f>
-        <v>0</v>
+        <v>15683.400000000373</v>
       </c>
       <c r="G132" s="2">
         <f>[1]NOVEMBER!$K$66</f>
-        <v>0</v>
+        <v>70.700000001117587</v>
       </c>
       <c r="H132" s="2">
         <f>[1]NOVEMBER!$L$66</f>
-        <v>0</v>
+        <v>412.69999999852735</v>
       </c>
       <c r="I132" s="2">
         <f>[1]NOVEMBER!$N$66</f>
-        <v>0</v>
+        <v>4434.0000000003211</v>
       </c>
       <c r="J132" s="2">
         <f>[1]NOVEMBER!$P$66</f>
@@ -17848,11 +17404,11 @@
       </c>
       <c r="M132" s="2">
         <f>[1]NOVEMBER!$T$66</f>
-        <v>0</v>
+        <v>17.069999999999709</v>
       </c>
       <c r="N132" s="2">
-        <f>[1]NOVEMBER!$Z$66</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$66</f>
+        <v>1330</v>
       </c>
       <c r="O132" s="2">
         <f>[1]NOVEMBER!$V$66</f>
@@ -17899,19 +17455,19 @@
       </c>
       <c r="F133" s="2">
         <f>[1]NOVEMBER!$J$67</f>
-        <v>0</v>
+        <v>15453.099999999627</v>
       </c>
       <c r="G133" s="2">
         <f>[1]NOVEMBER!$K$67</f>
-        <v>0</v>
+        <v>144.09999999962747</v>
       </c>
       <c r="H133" s="2">
         <f>[1]NOVEMBER!$L$67</f>
-        <v>0</v>
+        <v>508.9999999998181</v>
       </c>
       <c r="I133" s="2">
         <f>[1]NOVEMBER!$N$67</f>
-        <v>0</v>
+        <v>4373.0000000001828</v>
       </c>
       <c r="J133" s="2">
         <f>[1]NOVEMBER!$P$67</f>
@@ -17927,11 +17483,11 @@
       </c>
       <c r="M133" s="2">
         <f>[1]NOVEMBER!$T$67</f>
-        <v>0</v>
+        <v>17.090000000000146</v>
       </c>
       <c r="N133" s="2">
-        <f>[1]NOVEMBER!$Z$67</f>
-        <v>744</v>
+        <f>[1]NOVEMBER!$H$67</f>
+        <v>1330</v>
       </c>
       <c r="O133" s="2">
         <f>[1]NOVEMBER!$V$67</f>
@@ -17958,14 +17514,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>2021</v>
       </c>
-      <c r="B134">
+      <c r="B134" s="1">
         <v>12</v>
       </c>
-      <c r="C134" t="s">
+      <c r="C134" s="1" t="s">
         <v>18</v>
       </c>
       <c r="D134" s="2">
@@ -18009,8 +17565,8 @@
         <v>0</v>
       </c>
       <c r="N134" s="2">
-        <f>[1]DESEMBER!$Z$56</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$56</f>
+        <v>500</v>
       </c>
       <c r="O134" s="2">
         <f>[1]DESEMBER!$V$56</f>
@@ -18037,14 +17593,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>2021</v>
       </c>
-      <c r="B135">
+      <c r="B135" s="1">
         <v>12</v>
       </c>
-      <c r="C135" t="s">
+      <c r="C135" s="1" t="s">
         <v>20</v>
       </c>
       <c r="D135" s="2">
@@ -18088,8 +17644,8 @@
         <v>0</v>
       </c>
       <c r="N135" s="2">
-        <f>[1]DESEMBER!$Z$57</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$57</f>
+        <v>500</v>
       </c>
       <c r="O135" s="2">
         <f>[1]DESEMBER!$V$57</f>
@@ -18116,14 +17672,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="136" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="136" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A136">
         <v>2021</v>
       </c>
-      <c r="B136">
+      <c r="B136" s="1">
         <v>12</v>
       </c>
-      <c r="C136" t="s">
+      <c r="C136" s="1" t="s">
         <v>19</v>
       </c>
       <c r="D136" s="2">
@@ -18167,8 +17723,8 @@
         <v>0</v>
       </c>
       <c r="N136" s="2">
-        <f>[1]DESEMBER!$Z$58</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$58</f>
+        <v>1000</v>
       </c>
       <c r="O136" s="2">
         <f>[1]DESEMBER!$V$58</f>
@@ -18195,14 +17751,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="137" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="137" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A137">
         <v>2021</v>
       </c>
-      <c r="B137">
+      <c r="B137" s="1">
         <v>12</v>
       </c>
-      <c r="C137" t="s">
+      <c r="C137" s="1" t="s">
         <v>21</v>
       </c>
       <c r="D137" s="2">
@@ -18246,7 +17802,7 @@
         <v>0</v>
       </c>
       <c r="N137" s="2">
-        <f>[1]DESEMBER!$Z$59</f>
+        <f>[1]DESEMBER!$H$59</f>
         <v>0</v>
       </c>
       <c r="O137" s="2">
@@ -18274,14 +17830,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="138" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="138" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A138">
         <v>2021</v>
       </c>
-      <c r="B138">
+      <c r="B138" s="1">
         <v>12</v>
       </c>
-      <c r="C138" t="s">
+      <c r="C138" s="1" t="s">
         <v>22</v>
       </c>
       <c r="D138" s="2">
@@ -18325,8 +17881,8 @@
         <v>22.383333333333329</v>
       </c>
       <c r="N138" s="2">
-        <f>[1]DESEMBER!$Z$60</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$60</f>
+        <v>2500</v>
       </c>
       <c r="O138" s="2">
         <f>[1]DESEMBER!$V$60</f>
@@ -18353,14 +17909,14 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="139" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A139">
         <v>2021</v>
       </c>
-      <c r="B139">
+      <c r="B139" s="1">
         <v>12</v>
       </c>
-      <c r="C139" t="s">
+      <c r="C139" s="1" t="s">
         <v>23</v>
       </c>
       <c r="D139" s="2">
@@ -18404,8 +17960,8 @@
         <v>21.79999999999999</v>
       </c>
       <c r="N139" s="2">
-        <f>[1]DESEMBER!$Z$61</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$61</f>
+        <v>2500</v>
       </c>
       <c r="O139" s="2">
         <f>[1]DESEMBER!$V$61</f>
@@ -18432,11 +17988,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="140" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="140" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A140">
         <v>2021</v>
       </c>
-      <c r="B140">
+      <c r="B140" s="1">
         <v>12</v>
       </c>
       <c r="C140" s="1" t="s">
@@ -18444,11 +18000,11 @@
       </c>
       <c r="D140" s="2">
         <f>[1]DESEMBER!$H$62</f>
-        <v>1330</v>
+        <v>0</v>
       </c>
       <c r="E140" s="2">
         <f>[1]DESEMBER!$I$62</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F140" s="2">
         <f>[1]DESEMBER!$J$62</f>
@@ -18483,8 +18039,8 @@
         <v>0</v>
       </c>
       <c r="N140" s="2">
-        <f>[1]DESEMBER!$Z$62</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$62</f>
+        <v>0</v>
       </c>
       <c r="O140" s="2">
         <f>[1]DESEMBER!$V$62</f>
@@ -18511,11 +18067,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="141" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="141" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A141">
         <v>2021</v>
       </c>
-      <c r="B141">
+      <c r="B141" s="1">
         <v>12</v>
       </c>
       <c r="C141" s="1" t="s">
@@ -18523,11 +18079,11 @@
       </c>
       <c r="D141" s="2">
         <f>[1]DESEMBER!$H$63</f>
-        <v>1330</v>
+        <v>0</v>
       </c>
       <c r="E141" s="2">
         <f>[1]DESEMBER!$I$63</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F141" s="2">
         <f>[1]DESEMBER!$J$63</f>
@@ -18562,8 +18118,8 @@
         <v>0</v>
       </c>
       <c r="N141" s="2">
-        <f>[1]DESEMBER!$Z$63</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$63</f>
+        <v>0</v>
       </c>
       <c r="O141" s="2">
         <f>[1]DESEMBER!$V$63</f>
@@ -18590,11 +18146,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="142" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="142" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A142">
         <v>2021</v>
       </c>
-      <c r="B142">
+      <c r="B142" s="1">
         <v>12</v>
       </c>
       <c r="C142" s="1" t="s">
@@ -18602,11 +18158,11 @@
       </c>
       <c r="D142" s="2">
         <f>[1]DESEMBER!$H$64</f>
-        <v>1330</v>
+        <v>0</v>
       </c>
       <c r="E142" s="2">
         <f>[1]DESEMBER!$I$64</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F142" s="2">
         <f>[1]DESEMBER!$J$64</f>
@@ -18641,8 +18197,8 @@
         <v>0</v>
       </c>
       <c r="N142" s="2">
-        <f>[1]DESEMBER!$Z$64</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$64</f>
+        <v>0</v>
       </c>
       <c r="O142" s="2">
         <f>[1]DESEMBER!$V$64</f>
@@ -18669,11 +18225,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="143" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="143" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A143">
         <v>2021</v>
       </c>
-      <c r="B143">
+      <c r="B143" s="1">
         <v>12</v>
       </c>
       <c r="C143" s="1" t="s">
@@ -18681,11 +18237,11 @@
       </c>
       <c r="D143" s="2">
         <f>[1]DESEMBER!$H$65</f>
-        <v>1330</v>
+        <v>0</v>
       </c>
       <c r="E143" s="2">
         <f>[1]DESEMBER!$I$65</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F143" s="2">
         <f>[1]DESEMBER!$J$65</f>
@@ -18720,8 +18276,8 @@
         <v>0</v>
       </c>
       <c r="N143" s="2">
-        <f>[1]DESEMBER!$Z$65</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$65</f>
+        <v>0</v>
       </c>
       <c r="O143" s="2">
         <f>[1]DESEMBER!$V$65</f>
@@ -18748,11 +18304,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="144" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="144" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A144">
         <v>2021</v>
       </c>
-      <c r="B144">
+      <c r="B144" s="1">
         <v>12</v>
       </c>
       <c r="C144" s="1" t="s">
@@ -18760,11 +18316,11 @@
       </c>
       <c r="D144" s="2">
         <f>[1]DESEMBER!$H$66</f>
-        <v>1330</v>
+        <v>0</v>
       </c>
       <c r="E144" s="2">
         <f>[1]DESEMBER!$I$66</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F144" s="2">
         <f>[1]DESEMBER!$J$66</f>
@@ -18799,8 +18355,8 @@
         <v>0</v>
       </c>
       <c r="N144" s="2">
-        <f>[1]DESEMBER!$Z$66</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$66</f>
+        <v>0</v>
       </c>
       <c r="O144" s="2">
         <f>[1]DESEMBER!$V$66</f>
@@ -18827,11 +18383,11 @@
         <v>0</v>
       </c>
     </row>
-    <row r="145" spans="1:20" x14ac:dyDescent="0.3">
+    <row r="145" spans="1:20" s="1" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A145">
         <v>2021</v>
       </c>
-      <c r="B145">
+      <c r="B145" s="1">
         <v>12</v>
       </c>
       <c r="C145" s="1" t="s">
@@ -18839,11 +18395,11 @@
       </c>
       <c r="D145" s="2">
         <f>[1]DESEMBER!$H$67</f>
-        <v>1330</v>
+        <v>0</v>
       </c>
       <c r="E145" s="2">
         <f>[1]DESEMBER!$I$67</f>
-        <v>1000</v>
+        <v>0</v>
       </c>
       <c r="F145" s="2">
         <f>[1]DESEMBER!$J$67</f>
@@ -18878,8 +18434,8 @@
         <v>0</v>
       </c>
       <c r="N145" s="2">
-        <f>[1]DESEMBER!$Z$67</f>
-        <v>744</v>
+        <f>[1]DESEMBER!$H$67</f>
+        <v>0</v>
       </c>
       <c r="O145" s="2">
         <f>[1]DESEMBER!$V$67</f>

</xml_diff>